<commit_message>
Fixed Sudan in country mapping
</commit_message>
<xml_diff>
--- a/Data Management/Mappings/CountryIncomeCategory.xlsx
+++ b/Data Management/Mappings/CountryIncomeCategory.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14117" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14118" uniqueCount="976">
   <si>
     <t>Document:</t>
   </si>
@@ -3147,10 +3147,17 @@
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
     <numFmt numFmtId="165" formatCode="General_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -3317,18 +3324,18 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="40" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="40" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3343,39 +3350,39 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3385,34 +3392,34 @@
     <xf numFmtId="40" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3424,42 +3431,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3468,31 +3475,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -6451,10 +6459,10 @@
   <dimension ref="A1:IW240"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="10" topLeftCell="Z11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="10" topLeftCell="Z179" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AA5" sqref="AA5"/>
+      <selection pane="bottomRight" activeCell="C190" sqref="C190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.25"/>
@@ -26583,9 +26591,9 @@
       <c r="A190" s="24" t="s">
         <v>826</v>
       </c>
-      <c r="B190" s="74" t="str">
+      <c r="B190" s="74" t="e">
         <f>VLOOKUP(C190,UKB_CountryNames!B:C,2,FALSE)</f>
-        <v>Sudan</v>
+        <v>#N/A</v>
       </c>
       <c r="C190" s="25" t="s">
         <v>827</v>
@@ -27339,9 +27347,9 @@
       <c r="A197" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="B197" s="74" t="e">
+      <c r="B197" s="74" t="str">
         <f>VLOOKUP(C197,UKB_CountryNames!B:C,2,FALSE)</f>
-        <v>#N/A</v>
+        <v>Sudan</v>
       </c>
       <c r="C197" s="25" t="s">
         <v>94</v>
@@ -31641,8 +31649,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
+      <selection activeCell="C191" sqref="C191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35926,16 +35934,15 @@
       <c r="A174" s="71">
         <v>144</v>
       </c>
-      <c r="B174" s="71" t="str">
-        <f>VLOOKUP("*"&amp;C174&amp;"*",'Country Analytical History'!C:K,1,FALSE)</f>
-        <v>South Sudan</v>
+      <c r="B174" s="82" t="s">
+        <v>94</v>
       </c>
       <c r="C174" s="71" t="s">
         <v>94</v>
       </c>
       <c r="D174" s="71" t="str">
         <f>VLOOKUP(B174,'Country Analytical History'!C:AA,25,FALSE)</f>
-        <v>..</v>
+        <v>LM</v>
       </c>
       <c r="E174" s="71">
         <v>144</v>

</xml_diff>